<commit_message>
Add config and cli
</commit_message>
<xml_diff>
--- a/tests/fixtures/journal.xlsx
+++ b/tests/fixtures/journal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varch\Git-repos\brightsidebudget\tests\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DD5CC7-6ADA-4FD4-ACED-3FF40229E60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147BD9B5-58B8-4413-BC18-2BEF587445B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28620" yWindow="615" windowWidth="27247" windowHeight="14723" activeTab="2" xr2:uid="{B75559DA-6894-40C1-A499-6DBBA607E41C}"/>
+    <workbookView xWindow="1118" yWindow="383" windowWidth="27247" windowHeight="14722" activeTab="2" xr2:uid="{B75559DA-6894-40C1-A499-6DBBA607E41C}"/>
   </bookViews>
   <sheets>
     <sheet name="Comptes" sheetId="1" r:id="rId1"/>
@@ -751,7 +751,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" activeCellId="1" sqref="D2 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -886,7 +886,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -919,7 +919,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>1499.99</v>
+        <v>1499.9</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Simplified repository and extra columns
</commit_message>
<xml_diff>
--- a/tests/fixtures/journal.xlsx
+++ b/tests/fixtures/journal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varch\Git-repos\brightsidebudget\tests\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147BD9B5-58B8-4413-BC18-2BEF587445B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84729427-2A78-4D46-AC2C-C4A7A05969F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1118" yWindow="383" windowWidth="27247" windowHeight="14722" activeTab="2" xr2:uid="{B75559DA-6894-40C1-A499-6DBBA607E41C}"/>
+    <workbookView xWindow="-25493" yWindow="1215" windowWidth="23836" windowHeight="12128" activeTab="2" xr2:uid="{B75559DA-6894-40C1-A499-6DBBA607E41C}"/>
   </bookViews>
   <sheets>
     <sheet name="Comptes" sheetId="1" r:id="rId1"/>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A5AF20D-94EF-4EFB-9173-AC33D07B03BF}" name="Table1" displayName="Table1" ref="A1:E13" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A5AF20D-94EF-4EFB-9173-AC33D07B03BF}" name="Comptes" displayName="Comptes" ref="A1:E13" totalsRowShown="0">
   <autoFilter ref="A1:E13" xr:uid="{6A5AF20D-94EF-4EFB-9173-AC33D07B03BF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E5">
     <sortCondition ref="B2:B5"/>
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9E2078A3-4B09-463F-A4AC-4919F50A33B1}" name="Table2" displayName="Table2" ref="A1:G5" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9E2078A3-4B09-463F-A4AC-4919F50A33B1}" name="Txns" displayName="Txns" ref="A1:G5" totalsRowShown="0">
   <autoFilter ref="A1:G5" xr:uid="{9E2078A3-4B09-463F-A4AC-4919F50A33B1}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CD201035-C90D-4F14-AF69-041165CD75A1}" name="No txn"/>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D173D5C0-CEAA-485B-93A8-EED6FE761392}" name="Table3" displayName="Table3" ref="A1:D2" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D173D5C0-CEAA-485B-93A8-EED6FE761392}" name="Soldes" displayName="Soldes" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{D173D5C0-CEAA-485B-93A8-EED6FE761392}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D97E2C44-53BC-4479-ADE0-5E1181E31DEB}" name="Date" dataDxfId="0"/>
@@ -572,7 +572,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -751,7 +751,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D4" activeCellId="1" sqref="D2 D4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -886,7 +886,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Remove Non classée as account type
</commit_message>
<xml_diff>
--- a/tests/fixtures/journal.xlsx
+++ b/tests/fixtures/journal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varch\Git-repos\brightsidebudget\tests\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84729427-2A78-4D46-AC2C-C4A7A05969F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B005DF58-3ECD-4B96-9959-4D9925E0D32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25493" yWindow="1215" windowWidth="23836" windowHeight="12128" activeTab="2" xr2:uid="{B75559DA-6894-40C1-A499-6DBBA607E41C}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{B75559DA-6894-40C1-A499-6DBBA607E41C}"/>
   </bookViews>
   <sheets>
     <sheet name="Comptes" sheetId="1" r:id="rId1"/>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AB3DFD5-64F7-4D87-88A0-822B3E79FB03}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -732,10 +732,10 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13">
-        <v>6001</v>
+        <v>5999</v>
       </c>
     </row>
   </sheetData>
@@ -885,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59718142-3F44-47A1-A465-82EECCF10738}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>